<commit_message>
minor revision on scripts
</commit_message>
<xml_diff>
--- a/scripts/python/20countryXyear.xlsx
+++ b/scripts/python/20countryXyear.xlsx
@@ -465,7 +465,7 @@
         <v>2016</v>
       </c>
       <c r="C2">
-        <v>452</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -476,7 +476,7 @@
         <v>2017</v>
       </c>
       <c r="C3">
-        <v>323</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -487,7 +487,7 @@
         <v>2018</v>
       </c>
       <c r="C4">
-        <v>348</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -498,7 +498,7 @@
         <v>2019</v>
       </c>
       <c r="C5">
-        <v>344</v>
+        <v>381</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -509,7 +509,7 @@
         <v>2020</v>
       </c>
       <c r="C6">
-        <v>385</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -520,7 +520,7 @@
         <v>2021</v>
       </c>
       <c r="C7">
-        <v>290</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -531,7 +531,7 @@
         <v>2022</v>
       </c>
       <c r="C8">
-        <v>354</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -542,7 +542,7 @@
         <v>2023</v>
       </c>
       <c r="C9">
-        <v>247</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -553,7 +553,7 @@
         <v>2024</v>
       </c>
       <c r="C10">
-        <v>369</v>
+        <v>462</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -564,7 +564,7 @@
         <v>2016</v>
       </c>
       <c r="C11">
-        <v>56</v>
+        <v>439</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -575,7 +575,7 @@
         <v>2017</v>
       </c>
       <c r="C12">
-        <v>360</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -586,7 +586,7 @@
         <v>2018</v>
       </c>
       <c r="C13">
-        <v>259</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -597,7 +597,7 @@
         <v>2019</v>
       </c>
       <c r="C14">
-        <v>179</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -608,7 +608,7 @@
         <v>2020</v>
       </c>
       <c r="C15">
-        <v>263</v>
+        <v>405</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -619,7 +619,7 @@
         <v>2021</v>
       </c>
       <c r="C16">
-        <v>171</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -630,7 +630,7 @@
         <v>2022</v>
       </c>
       <c r="C17">
-        <v>93</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -641,7 +641,7 @@
         <v>2023</v>
       </c>
       <c r="C18">
-        <v>56</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -652,7 +652,7 @@
         <v>2024</v>
       </c>
       <c r="C19">
-        <v>178</v>
+        <v>363</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -663,7 +663,7 @@
         <v>2016</v>
       </c>
       <c r="C20">
-        <v>434</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -674,7 +674,7 @@
         <v>2017</v>
       </c>
       <c r="C21">
-        <v>190</v>
+        <v>443</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -685,7 +685,7 @@
         <v>2018</v>
       </c>
       <c r="C22">
-        <v>128</v>
+        <v>497</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -696,7 +696,7 @@
         <v>2019</v>
       </c>
       <c r="C23">
-        <v>76</v>
+        <v>407</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -707,7 +707,7 @@
         <v>2020</v>
       </c>
       <c r="C24">
-        <v>274</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -718,7 +718,7 @@
         <v>2021</v>
       </c>
       <c r="C25">
-        <v>483</v>
+        <v>431</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -729,7 +729,7 @@
         <v>2022</v>
       </c>
       <c r="C26">
-        <v>186</v>
+        <v>464</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -740,7 +740,7 @@
         <v>2023</v>
       </c>
       <c r="C27">
-        <v>388</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -751,7 +751,7 @@
         <v>2024</v>
       </c>
       <c r="C28">
-        <v>67</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -762,7 +762,7 @@
         <v>2016</v>
       </c>
       <c r="C29">
-        <v>357</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -773,7 +773,7 @@
         <v>2017</v>
       </c>
       <c r="C30">
-        <v>434</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -784,7 +784,7 @@
         <v>2018</v>
       </c>
       <c r="C31">
-        <v>332</v>
+        <v>446</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -795,7 +795,7 @@
         <v>2019</v>
       </c>
       <c r="C32">
-        <v>210</v>
+        <v>394</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -806,7 +806,7 @@
         <v>2020</v>
       </c>
       <c r="C33">
-        <v>387</v>
+        <v>446</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -817,7 +817,7 @@
         <v>2021</v>
       </c>
       <c r="C34">
-        <v>332</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -828,7 +828,7 @@
         <v>2022</v>
       </c>
       <c r="C35">
-        <v>410</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -839,7 +839,7 @@
         <v>2023</v>
       </c>
       <c r="C36">
-        <v>274</v>
+        <v>429</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -850,7 +850,7 @@
         <v>2024</v>
       </c>
       <c r="C37">
-        <v>236</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -861,7 +861,7 @@
         <v>2016</v>
       </c>
       <c r="C38">
-        <v>497</v>
+        <v>392</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -872,7 +872,7 @@
         <v>2017</v>
       </c>
       <c r="C39">
-        <v>113</v>
+        <v>356</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -883,7 +883,7 @@
         <v>2018</v>
       </c>
       <c r="C40">
-        <v>314</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -894,7 +894,7 @@
         <v>2019</v>
       </c>
       <c r="C41">
-        <v>432</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -905,7 +905,7 @@
         <v>2020</v>
       </c>
       <c r="C42">
-        <v>379</v>
+        <v>311</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -916,7 +916,7 @@
         <v>2021</v>
       </c>
       <c r="C43">
-        <v>143</v>
+        <v>459</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -927,7 +927,7 @@
         <v>2022</v>
       </c>
       <c r="C44">
-        <v>329</v>
+        <v>474</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -938,7 +938,7 @@
         <v>2023</v>
       </c>
       <c r="C45">
-        <v>387</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -949,7 +949,7 @@
         <v>2024</v>
       </c>
       <c r="C46">
-        <v>255</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -960,7 +960,7 @@
         <v>2016</v>
       </c>
       <c r="C47">
-        <v>219</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -971,7 +971,7 @@
         <v>2017</v>
       </c>
       <c r="C48">
-        <v>74</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -982,7 +982,7 @@
         <v>2018</v>
       </c>
       <c r="C49">
-        <v>100</v>
+        <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -993,7 +993,7 @@
         <v>2019</v>
       </c>
       <c r="C50">
-        <v>50</v>
+        <v>475</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1004,7 +1004,7 @@
         <v>2020</v>
       </c>
       <c r="C51">
-        <v>345</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1015,7 +1015,7 @@
         <v>2021</v>
       </c>
       <c r="C52">
-        <v>328</v>
+        <v>490</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1026,7 +1026,7 @@
         <v>2022</v>
       </c>
       <c r="C53">
-        <v>185</v>
+        <v>341</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1037,7 +1037,7 @@
         <v>2023</v>
       </c>
       <c r="C54">
-        <v>347</v>
+        <v>444</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1048,7 +1048,7 @@
         <v>2024</v>
       </c>
       <c r="C55">
-        <v>364</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1059,7 +1059,7 @@
         <v>2016</v>
       </c>
       <c r="C56">
-        <v>289</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1070,7 +1070,7 @@
         <v>2017</v>
       </c>
       <c r="C57">
-        <v>337</v>
+        <v>250</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1081,7 +1081,7 @@
         <v>2018</v>
       </c>
       <c r="C58">
-        <v>303</v>
+        <v>440</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1092,7 +1092,7 @@
         <v>2019</v>
       </c>
       <c r="C59">
-        <v>498</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1103,7 +1103,7 @@
         <v>2020</v>
       </c>
       <c r="C60">
-        <v>340</v>
+        <v>353</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1114,7 +1114,7 @@
         <v>2021</v>
       </c>
       <c r="C61">
-        <v>86</v>
+        <v>261</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1125,7 +1125,7 @@
         <v>2022</v>
       </c>
       <c r="C62">
-        <v>445</v>
+        <v>296</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1136,7 +1136,7 @@
         <v>2023</v>
       </c>
       <c r="C63">
-        <v>170</v>
+        <v>454</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1147,7 +1147,7 @@
         <v>2024</v>
       </c>
       <c r="C64">
-        <v>403</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1158,7 +1158,7 @@
         <v>2016</v>
       </c>
       <c r="C65">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1169,7 +1169,7 @@
         <v>2017</v>
       </c>
       <c r="C66">
-        <v>318</v>
+        <v>475</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1180,7 +1180,7 @@
         <v>2018</v>
       </c>
       <c r="C67">
-        <v>322</v>
+        <v>337</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1191,7 +1191,7 @@
         <v>2019</v>
       </c>
       <c r="C68">
-        <v>147</v>
+        <v>479</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1202,7 +1202,7 @@
         <v>2020</v>
       </c>
       <c r="C69">
-        <v>493</v>
+        <v>371</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1213,7 +1213,7 @@
         <v>2021</v>
       </c>
       <c r="C70">
-        <v>313</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1235,7 +1235,7 @@
         <v>2023</v>
       </c>
       <c r="C72">
-        <v>499</v>
+        <v>311</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1246,7 +1246,7 @@
         <v>2024</v>
       </c>
       <c r="C73">
-        <v>473</v>
+        <v>181</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1257,7 +1257,7 @@
         <v>2016</v>
       </c>
       <c r="C74">
-        <v>158</v>
+        <v>83</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1268,7 +1268,7 @@
         <v>2017</v>
       </c>
       <c r="C75">
-        <v>377</v>
+        <v>166</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1279,7 +1279,7 @@
         <v>2018</v>
       </c>
       <c r="C76">
-        <v>136</v>
+        <v>301</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1290,7 +1290,7 @@
         <v>2019</v>
       </c>
       <c r="C77">
-        <v>417</v>
+        <v>484</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1301,7 +1301,7 @@
         <v>2020</v>
       </c>
       <c r="C78">
-        <v>328</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1312,7 +1312,7 @@
         <v>2021</v>
       </c>
       <c r="C79">
-        <v>59</v>
+        <v>219</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1323,7 +1323,7 @@
         <v>2022</v>
       </c>
       <c r="C80">
-        <v>462</v>
+        <v>388</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1334,7 +1334,7 @@
         <v>2023</v>
       </c>
       <c r="C81">
-        <v>179</v>
+        <v>301</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1345,7 +1345,7 @@
         <v>2024</v>
       </c>
       <c r="C82">
-        <v>306</v>
+        <v>316</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1356,7 +1356,7 @@
         <v>2016</v>
       </c>
       <c r="C83">
-        <v>292</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1367,7 +1367,7 @@
         <v>2017</v>
       </c>
       <c r="C84">
-        <v>486</v>
+        <v>186</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1378,7 +1378,7 @@
         <v>2018</v>
       </c>
       <c r="C85">
-        <v>192</v>
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1389,7 +1389,7 @@
         <v>2019</v>
       </c>
       <c r="C86">
-        <v>274</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1400,7 +1400,7 @@
         <v>2020</v>
       </c>
       <c r="C87">
-        <v>456</v>
+        <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1411,7 +1411,7 @@
         <v>2021</v>
       </c>
       <c r="C88">
-        <v>438</v>
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1422,7 +1422,7 @@
         <v>2022</v>
       </c>
       <c r="C89">
-        <v>405</v>
+        <v>465</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1433,7 +1433,7 @@
         <v>2023</v>
       </c>
       <c r="C90">
-        <v>274</v>
+        <v>298</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1444,7 +1444,7 @@
         <v>2024</v>
       </c>
       <c r="C91">
-        <v>137</v>
+        <v>156</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1455,7 +1455,7 @@
         <v>2016</v>
       </c>
       <c r="C92">
-        <v>273</v>
+        <v>397</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1466,7 +1466,7 @@
         <v>2017</v>
       </c>
       <c r="C93">
-        <v>417</v>
+        <v>206</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1477,7 +1477,7 @@
         <v>2018</v>
       </c>
       <c r="C94">
-        <v>126</v>
+        <v>144</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1488,7 +1488,7 @@
         <v>2019</v>
       </c>
       <c r="C95">
-        <v>231</v>
+        <v>492</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1499,7 +1499,7 @@
         <v>2020</v>
       </c>
       <c r="C96">
-        <v>251</v>
+        <v>435</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1510,7 +1510,7 @@
         <v>2021</v>
       </c>
       <c r="C97">
-        <v>134</v>
+        <v>359</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1521,7 +1521,7 @@
         <v>2022</v>
       </c>
       <c r="C98">
-        <v>245</v>
+        <v>444</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1532,7 +1532,7 @@
         <v>2023</v>
       </c>
       <c r="C99">
-        <v>320</v>
+        <v>87</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1543,7 +1543,7 @@
         <v>2024</v>
       </c>
       <c r="C100">
-        <v>50</v>
+        <v>462</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1554,7 +1554,7 @@
         <v>2016</v>
       </c>
       <c r="C101">
-        <v>277</v>
+        <v>172</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1565,7 +1565,7 @@
         <v>2017</v>
       </c>
       <c r="C102">
-        <v>124</v>
+        <v>248</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1576,7 +1576,7 @@
         <v>2018</v>
       </c>
       <c r="C103">
-        <v>418</v>
+        <v>462</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1587,7 +1587,7 @@
         <v>2019</v>
       </c>
       <c r="C104">
-        <v>273</v>
+        <v>136</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -1598,7 +1598,7 @@
         <v>2020</v>
       </c>
       <c r="C105">
-        <v>300</v>
+        <v>471</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -1609,7 +1609,7 @@
         <v>2021</v>
       </c>
       <c r="C106">
-        <v>252</v>
+        <v>228</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -1620,7 +1620,7 @@
         <v>2022</v>
       </c>
       <c r="C107">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -1631,7 +1631,7 @@
         <v>2023</v>
       </c>
       <c r="C108">
-        <v>368</v>
+        <v>304</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -1642,7 +1642,7 @@
         <v>2024</v>
       </c>
       <c r="C109">
-        <v>95</v>
+        <v>241</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -1653,7 +1653,7 @@
         <v>2016</v>
       </c>
       <c r="C110">
-        <v>220</v>
+        <v>417</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -1664,7 +1664,7 @@
         <v>2017</v>
       </c>
       <c r="C111">
-        <v>66</v>
+        <v>240</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -1675,7 +1675,7 @@
         <v>2018</v>
       </c>
       <c r="C112">
-        <v>66</v>
+        <v>268</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -1686,7 +1686,7 @@
         <v>2019</v>
       </c>
       <c r="C113">
-        <v>495</v>
+        <v>92</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -1697,7 +1697,7 @@
         <v>2020</v>
       </c>
       <c r="C114">
-        <v>490</v>
+        <v>91</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -1708,7 +1708,7 @@
         <v>2021</v>
       </c>
       <c r="C115">
-        <v>72</v>
+        <v>196</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -1719,7 +1719,7 @@
         <v>2022</v>
       </c>
       <c r="C116">
-        <v>239</v>
+        <v>495</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -1730,7 +1730,7 @@
         <v>2023</v>
       </c>
       <c r="C117">
-        <v>477</v>
+        <v>335</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -1741,7 +1741,7 @@
         <v>2024</v>
       </c>
       <c r="C118">
-        <v>247</v>
+        <v>339</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -1752,7 +1752,7 @@
         <v>2016</v>
       </c>
       <c r="C119">
-        <v>300</v>
+        <v>399</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -1763,7 +1763,7 @@
         <v>2017</v>
       </c>
       <c r="C120">
-        <v>311</v>
+        <v>415</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -1774,7 +1774,7 @@
         <v>2018</v>
       </c>
       <c r="C121">
-        <v>152</v>
+        <v>362</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -1785,7 +1785,7 @@
         <v>2019</v>
       </c>
       <c r="C122">
-        <v>143</v>
+        <v>244</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -1796,7 +1796,7 @@
         <v>2020</v>
       </c>
       <c r="C123">
-        <v>205</v>
+        <v>460</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -1807,7 +1807,7 @@
         <v>2021</v>
       </c>
       <c r="C124">
-        <v>190</v>
+        <v>456</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -1818,7 +1818,7 @@
         <v>2022</v>
       </c>
       <c r="C125">
-        <v>140</v>
+        <v>485</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -1829,7 +1829,7 @@
         <v>2023</v>
       </c>
       <c r="C126">
-        <v>413</v>
+        <v>221</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -1840,7 +1840,7 @@
         <v>2024</v>
       </c>
       <c r="C127">
-        <v>492</v>
+        <v>442</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -1851,7 +1851,7 @@
         <v>2016</v>
       </c>
       <c r="C128">
-        <v>156</v>
+        <v>453</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -1862,7 +1862,7 @@
         <v>2017</v>
       </c>
       <c r="C129">
-        <v>349</v>
+        <v>271</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -1873,7 +1873,7 @@
         <v>2018</v>
       </c>
       <c r="C130">
-        <v>220</v>
+        <v>326</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -1884,7 +1884,7 @@
         <v>2019</v>
       </c>
       <c r="C131">
-        <v>394</v>
+        <v>260</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -1895,7 +1895,7 @@
         <v>2020</v>
       </c>
       <c r="C132">
-        <v>487</v>
+        <v>262</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -1906,7 +1906,7 @@
         <v>2021</v>
       </c>
       <c r="C133">
-        <v>63</v>
+        <v>276</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -1917,7 +1917,7 @@
         <v>2022</v>
       </c>
       <c r="C134">
-        <v>156</v>
+        <v>450</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -1928,7 +1928,7 @@
         <v>2023</v>
       </c>
       <c r="C135">
-        <v>179</v>
+        <v>200</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -1939,7 +1939,7 @@
         <v>2024</v>
       </c>
       <c r="C136">
-        <v>385</v>
+        <v>481</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -1950,7 +1950,7 @@
         <v>2016</v>
       </c>
       <c r="C137">
-        <v>294</v>
+        <v>248</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -1961,7 +1961,7 @@
         <v>2017</v>
       </c>
       <c r="C138">
-        <v>472</v>
+        <v>263</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -1972,7 +1972,7 @@
         <v>2018</v>
       </c>
       <c r="C139">
-        <v>89</v>
+        <v>63</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -1983,7 +1983,7 @@
         <v>2019</v>
       </c>
       <c r="C140">
-        <v>205</v>
+        <v>493</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -1994,7 +1994,7 @@
         <v>2020</v>
       </c>
       <c r="C141">
-        <v>191</v>
+        <v>207</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2005,7 +2005,7 @@
         <v>2021</v>
       </c>
       <c r="C142">
-        <v>301</v>
+        <v>73</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2016,7 +2016,7 @@
         <v>2022</v>
       </c>
       <c r="C143">
-        <v>354</v>
+        <v>279</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2027,7 +2027,7 @@
         <v>2023</v>
       </c>
       <c r="C144">
-        <v>136</v>
+        <v>202</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2038,7 +2038,7 @@
         <v>2024</v>
       </c>
       <c r="C145">
-        <v>342</v>
+        <v>309</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2049,7 +2049,7 @@
         <v>2016</v>
       </c>
       <c r="C146">
-        <v>479</v>
+        <v>383</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2060,7 +2060,7 @@
         <v>2017</v>
       </c>
       <c r="C147">
-        <v>353</v>
+        <v>443</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2071,7 +2071,7 @@
         <v>2018</v>
       </c>
       <c r="C148">
-        <v>67</v>
+        <v>211</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2082,7 +2082,7 @@
         <v>2019</v>
       </c>
       <c r="C149">
-        <v>76</v>
+        <v>210</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2093,7 +2093,7 @@
         <v>2020</v>
       </c>
       <c r="C150">
-        <v>126</v>
+        <v>63</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2104,7 +2104,7 @@
         <v>2021</v>
       </c>
       <c r="C151">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2115,7 +2115,7 @@
         <v>2022</v>
       </c>
       <c r="C152">
-        <v>79</v>
+        <v>281</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2126,7 +2126,7 @@
         <v>2023</v>
       </c>
       <c r="C153">
-        <v>438</v>
+        <v>430</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2137,7 +2137,7 @@
         <v>2024</v>
       </c>
       <c r="C154">
-        <v>417</v>
+        <v>349</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2148,7 +2148,7 @@
         <v>2016</v>
       </c>
       <c r="C155">
-        <v>447</v>
+        <v>157</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2159,7 +2159,7 @@
         <v>2017</v>
       </c>
       <c r="C156">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2170,7 +2170,7 @@
         <v>2018</v>
       </c>
       <c r="C157">
-        <v>469</v>
+        <v>220</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2181,7 +2181,7 @@
         <v>2019</v>
       </c>
       <c r="C158">
-        <v>356</v>
+        <v>310</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2192,7 +2192,7 @@
         <v>2020</v>
       </c>
       <c r="C159">
-        <v>427</v>
+        <v>398</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2203,7 +2203,7 @@
         <v>2021</v>
       </c>
       <c r="C160">
-        <v>348</v>
+        <v>292</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2214,7 +2214,7 @@
         <v>2022</v>
       </c>
       <c r="C161">
-        <v>114</v>
+        <v>370</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2225,7 +2225,7 @@
         <v>2023</v>
       </c>
       <c r="C162">
-        <v>259</v>
+        <v>281</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2236,7 +2236,7 @@
         <v>2024</v>
       </c>
       <c r="C163">
-        <v>191</v>
+        <v>364</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2247,7 +2247,7 @@
         <v>2016</v>
       </c>
       <c r="C164">
-        <v>419</v>
+        <v>322</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2258,7 +2258,7 @@
         <v>2017</v>
       </c>
       <c r="C165">
-        <v>196</v>
+        <v>415</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2269,7 +2269,7 @@
         <v>2018</v>
       </c>
       <c r="C166">
-        <v>156</v>
+        <v>342</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2280,7 +2280,7 @@
         <v>2019</v>
       </c>
       <c r="C167">
-        <v>269</v>
+        <v>51</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2291,7 +2291,7 @@
         <v>2020</v>
       </c>
       <c r="C168">
-        <v>192</v>
+        <v>262</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2302,7 +2302,7 @@
         <v>2021</v>
       </c>
       <c r="C169">
-        <v>54</v>
+        <v>291</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2313,7 +2313,7 @@
         <v>2022</v>
       </c>
       <c r="C170">
-        <v>130</v>
+        <v>224</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2324,7 +2324,7 @@
         <v>2023</v>
       </c>
       <c r="C171">
-        <v>195</v>
+        <v>320</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2335,7 +2335,7 @@
         <v>2024</v>
       </c>
       <c r="C172">
-        <v>331</v>
+        <v>289</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2346,7 +2346,7 @@
         <v>2016</v>
       </c>
       <c r="C173">
-        <v>376</v>
+        <v>213</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2357,7 +2357,7 @@
         <v>2017</v>
       </c>
       <c r="C174">
-        <v>442</v>
+        <v>425</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2368,7 +2368,7 @@
         <v>2018</v>
       </c>
       <c r="C175">
-        <v>330</v>
+        <v>439</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2379,7 +2379,7 @@
         <v>2019</v>
       </c>
       <c r="C176">
-        <v>351</v>
+        <v>233</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2390,7 +2390,7 @@
         <v>2020</v>
       </c>
       <c r="C177">
-        <v>347</v>
+        <v>248</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2401,7 +2401,7 @@
         <v>2021</v>
       </c>
       <c r="C178">
-        <v>376</v>
+        <v>121</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -2412,7 +2412,7 @@
         <v>2022</v>
       </c>
       <c r="C179">
-        <v>196</v>
+        <v>114</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2423,7 +2423,7 @@
         <v>2023</v>
       </c>
       <c r="C180">
-        <v>210</v>
+        <v>365</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2434,7 +2434,7 @@
         <v>2024</v>
       </c>
       <c r="C181">
-        <v>432</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>